<commit_message>
Had not included species in the subplot data that weren't also in the master species list
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/01b_edited-species7_location-independent-final-fix.xlsx
+++ b/data/data-wrangling-intermediate/01b_edited-species7_location-independent-final-fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CC9AE79-41C4-4FFD-AFEE-57AA938EEAE0}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B904A98F-D6C6-43B0-B55D-9E3E64576122}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2096,7 +2096,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2236,18 +2236,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2597,13 +2585,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3066,8 +3053,8 @@
   <dimension ref="A1:F478"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A183" sqref="A183"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3594,7 +3581,7 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
@@ -7782,13 +7769,13 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B236" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
       <c r="C236" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="D236" t="s">
         <v>3</v>
@@ -7805,16 +7792,16 @@
         <v>138</v>
       </c>
       <c r="B237" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="C237" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D237" t="s">
         <v>3</v>
       </c>
       <c r="E237" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F237" t="s">
         <v>17</v>
@@ -7822,7 +7809,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B238" t="s">
         <v>132</v>
@@ -11724,7 +11711,7 @@
       <c r="A433" t="s">
         <v>659</v>
       </c>
-      <c r="B433" s="3" t="s">
+      <c r="B433" s="1" t="s">
         <v>668</v>
       </c>
       <c r="C433" t="s">

</xml_diff>

<commit_message>
Had to change ATCA/ATCA2 in edited-species7.csv also
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/01b_edited-species7_location-independent-final-fix.xlsx
+++ b/data/data-wrangling-intermediate/01b_edited-species7_location-independent-final-fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B76343F-C2F1-4702-8A8A-3485BD85EB74}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55426C6D-9E40-4EEB-893E-768BD9E3B44C}"/>
   <bookViews>
     <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="664">
   <si>
     <t>CodeOriginal</t>
   </si>
@@ -1898,9 +1898,6 @@
   </si>
   <si>
     <t>ATCA</t>
-  </si>
-  <si>
-    <t>Atriplex californica</t>
   </si>
   <si>
     <t>Aristida species between the northeast and southeast pits possibly an ARPU if not than seeded species cover would be 0%</t>
@@ -3041,8 +3038,8 @@
   <dimension ref="A1:F476"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A440" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A314" sqref="A314"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4300,10 +4297,10 @@
         <v>604</v>
       </c>
       <c r="B63" t="s">
-        <v>604</v>
+        <v>110</v>
       </c>
       <c r="C63" t="s">
-        <v>605</v>
+        <v>111</v>
       </c>
       <c r="D63" t="s">
         <v>3</v>
@@ -4312,7 +4309,7 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -4377,7 +4374,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B67" t="s">
         <v>59</v>
@@ -4597,7 +4594,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B78" t="s">
         <v>59</v>
@@ -4617,7 +4614,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B79" t="s">
         <v>132</v>
@@ -4637,7 +4634,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B80" t="s">
         <v>132</v>
@@ -4657,7 +4654,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B81" t="s">
         <v>132</v>
@@ -5557,13 +5554,13 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>609</v>
+      </c>
+      <c r="B126" t="s">
+        <v>609</v>
+      </c>
+      <c r="C126" t="s">
         <v>610</v>
-      </c>
-      <c r="B126" t="s">
-        <v>610</v>
-      </c>
-      <c r="C126" t="s">
-        <v>611</v>
       </c>
       <c r="D126" t="s">
         <v>3</v>
@@ -5597,7 +5594,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B128" t="s">
         <v>235</v>
@@ -5817,13 +5814,13 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>611</v>
+      </c>
+      <c r="B139" t="s">
+        <v>611</v>
+      </c>
+      <c r="C139" t="s">
         <v>612</v>
-      </c>
-      <c r="B139" t="s">
-        <v>612</v>
-      </c>
-      <c r="C139" t="s">
-        <v>613</v>
       </c>
       <c r="D139" t="s">
         <v>3</v>
@@ -5837,7 +5834,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B140" t="s">
         <v>239</v>
@@ -5997,10 +5994,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B148" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C148" t="s">
         <v>57</v>
@@ -6337,13 +6334,13 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>615</v>
+      </c>
+      <c r="B165" t="s">
+        <v>615</v>
+      </c>
+      <c r="C165" t="s">
         <v>616</v>
-      </c>
-      <c r="B165" t="s">
-        <v>616</v>
-      </c>
-      <c r="C165" t="s">
-        <v>617</v>
       </c>
       <c r="D165" t="s">
         <v>3</v>
@@ -6817,7 +6814,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B189" t="s">
         <v>59</v>
@@ -7337,13 +7334,13 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
+        <v>619</v>
+      </c>
+      <c r="B215" t="s">
+        <v>619</v>
+      </c>
+      <c r="C215" t="s">
         <v>620</v>
-      </c>
-      <c r="B215" t="s">
-        <v>620</v>
-      </c>
-      <c r="C215" t="s">
-        <v>621</v>
       </c>
       <c r="D215" t="s">
         <v>3</v>
@@ -7597,13 +7594,13 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
+        <v>621</v>
+      </c>
+      <c r="B228" t="s">
+        <v>621</v>
+      </c>
+      <c r="C228" t="s">
         <v>622</v>
-      </c>
-      <c r="B228" t="s">
-        <v>622</v>
-      </c>
-      <c r="C228" t="s">
-        <v>623</v>
       </c>
       <c r="D228" t="s">
         <v>3</v>
@@ -7797,13 +7794,13 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
+        <v>623</v>
+      </c>
+      <c r="B238" t="s">
+        <v>623</v>
+      </c>
+      <c r="C238" t="s">
         <v>624</v>
-      </c>
-      <c r="B238" t="s">
-        <v>624</v>
-      </c>
-      <c r="C238" t="s">
-        <v>625</v>
       </c>
       <c r="D238" t="s">
         <v>105</v>
@@ -7937,7 +7934,7 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B245" t="s">
         <v>409</v>
@@ -8437,7 +8434,7 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B270" t="s">
         <v>59</v>
@@ -8457,7 +8454,7 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B271" t="s">
         <v>120</v>
@@ -8477,7 +8474,7 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B272" t="s">
         <v>132</v>
@@ -8597,7 +8594,7 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B278" t="s">
         <v>59</v>
@@ -8617,7 +8614,7 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B279" t="s">
         <v>132</v>
@@ -8637,7 +8634,7 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B280" t="s">
         <v>132</v>
@@ -8697,7 +8694,7 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B283" t="s">
         <v>59</v>
@@ -8757,7 +8754,7 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B286" t="s">
         <v>59</v>
@@ -8777,7 +8774,7 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B287" t="s">
         <v>59</v>
@@ -8797,7 +8794,7 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B288" t="s">
         <v>277</v>
@@ -8817,7 +8814,7 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B289" t="s">
         <v>524</v>
@@ -8837,7 +8834,7 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B290" t="s">
         <v>59</v>
@@ -8857,7 +8854,7 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B291" t="s">
         <v>132</v>
@@ -8937,7 +8934,7 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B295" t="s">
         <v>59</v>
@@ -8957,7 +8954,7 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B296" t="s">
         <v>132</v>
@@ -8977,7 +8974,7 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B297" t="s">
         <v>474</v>
@@ -8997,7 +8994,7 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B298" t="s">
         <v>59</v>
@@ -9017,7 +9014,7 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B299" t="s">
         <v>132</v>
@@ -9037,7 +9034,7 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B300" t="s">
         <v>15</v>
@@ -9057,7 +9054,7 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B301" t="s">
         <v>59</v>
@@ -9077,7 +9074,7 @@
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B302" t="s">
         <v>59</v>
@@ -9097,7 +9094,7 @@
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B303" t="s">
         <v>132</v>
@@ -9157,7 +9154,7 @@
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B306" t="s">
         <v>59</v>
@@ -9177,7 +9174,7 @@
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B307" t="s">
         <v>132</v>
@@ -9317,7 +9314,7 @@
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B314" t="s">
         <v>120</v>
@@ -9337,7 +9334,7 @@
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B315" t="s">
         <v>15</v>
@@ -9357,7 +9354,7 @@
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B316" t="s">
         <v>59</v>
@@ -9377,7 +9374,7 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B317" t="s">
         <v>120</v>
@@ -9397,7 +9394,7 @@
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B318" t="s">
         <v>524</v>
@@ -9657,7 +9654,7 @@
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B331" t="s">
         <v>454</v>
@@ -9717,13 +9714,13 @@
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
+        <v>641</v>
+      </c>
+      <c r="B334" t="s">
+        <v>641</v>
+      </c>
+      <c r="C334" t="s">
         <v>642</v>
-      </c>
-      <c r="B334" t="s">
-        <v>642</v>
-      </c>
-      <c r="C334" t="s">
-        <v>643</v>
       </c>
       <c r="D334" t="s">
         <v>3</v>
@@ -10197,7 +10194,7 @@
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B358">
         <v>0</v>
@@ -10317,7 +10314,7 @@
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B364" t="s">
         <v>409</v>
@@ -10337,7 +10334,7 @@
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B365" t="s">
         <v>409</v>
@@ -10357,7 +10354,7 @@
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B366" t="s">
         <v>551</v>
@@ -10417,7 +10414,7 @@
     </row>
     <row r="369" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B369" t="s">
         <v>454</v>
@@ -10437,7 +10434,7 @@
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B370" t="s">
         <v>551</v>
@@ -10577,7 +10574,7 @@
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B377" t="s">
         <v>489</v>
@@ -10597,7 +10594,7 @@
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B378" t="s">
         <v>551</v>
@@ -10717,7 +10714,7 @@
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B384" t="s">
         <v>551</v>
@@ -10737,7 +10734,7 @@
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B385" t="s">
         <v>409</v>
@@ -10757,7 +10754,7 @@
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B386" t="s">
         <v>551</v>
@@ -10777,7 +10774,7 @@
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B387" t="s">
         <v>551</v>
@@ -10897,7 +10894,7 @@
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B393" t="s">
         <v>551</v>
@@ -11637,13 +11634,13 @@
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
+        <v>652</v>
+      </c>
+      <c r="B430" t="s">
+        <v>652</v>
+      </c>
+      <c r="C430" t="s">
         <v>653</v>
-      </c>
-      <c r="B430" t="s">
-        <v>653</v>
-      </c>
-      <c r="C430" t="s">
-        <v>654</v>
       </c>
       <c r="D430" t="s">
         <v>3</v>
@@ -11657,13 +11654,13 @@
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
+        <v>654</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="C431" t="s">
         <v>655</v>
-      </c>
-      <c r="B431" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="C431" t="s">
-        <v>656</v>
       </c>
       <c r="D431" t="s">
         <v>3</v>
@@ -11897,7 +11894,7 @@
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B443" t="s">
         <v>59</v>
@@ -12057,7 +12054,7 @@
     </row>
     <row r="451" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B451" t="s">
         <v>132</v>
@@ -12077,7 +12074,7 @@
     </row>
     <row r="452" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B452" t="s">
         <v>524</v>
@@ -12297,7 +12294,7 @@
     </row>
     <row r="463" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B463" t="s">
         <v>409</v>
@@ -12317,7 +12314,7 @@
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B464" t="s">
         <v>409</v>
@@ -12337,7 +12334,7 @@
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B465" t="s">
         <v>132</v>
@@ -12357,7 +12354,7 @@
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B466" t="s">
         <v>524</v>
@@ -12377,7 +12374,7 @@
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B467" t="s">
         <v>489</v>
@@ -12397,7 +12394,7 @@
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B468" t="s">
         <v>551</v>

</xml_diff>

<commit_message>
Change LILE to LILE3 (did not complete the fix in the last commit, had to add more code to fix the Code
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/01b_edited-species7_location-independent-final-fix.xlsx
+++ b/data/data-wrangling-intermediate/01b_edited-species7_location-independent-final-fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55426C6D-9E40-4EEB-893E-768BD9E3B44C}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38C0BF40-4CB2-44A3-B78C-F337D1B52EC6}"/>
   <bookViews>
-    <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38490" yWindow="3180" windowWidth="13860" windowHeight="7125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="663">
   <si>
     <t>CodeOriginal</t>
   </si>
@@ -1226,9 +1226,6 @@
   </si>
   <si>
     <t>LILE</t>
-  </si>
-  <si>
-    <t>Leptosiphon lemmonii</t>
   </si>
   <si>
     <t>LILE3</t>
@@ -3038,8 +3035,8 @@
   <dimension ref="A1:F476"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F223" sqref="F223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3254,7 +3251,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B11" t="s">
         <v>59</v>
@@ -3274,7 +3271,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B12" t="s">
         <v>132</v>
@@ -3294,7 +3291,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B13" t="s">
         <v>132</v>
@@ -3314,13 +3311,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>487</v>
+      </c>
+      <c r="B14" t="s">
         <v>488</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>489</v>
-      </c>
-      <c r="C14" t="s">
-        <v>490</v>
       </c>
       <c r="D14" t="s">
         <v>3</v>
@@ -3334,13 +3331,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B15" t="s">
+        <v>523</v>
+      </c>
+      <c r="C15" t="s">
         <v>524</v>
-      </c>
-      <c r="C15" t="s">
-        <v>525</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -3414,7 +3411,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B19" t="s">
         <v>59</v>
@@ -3434,13 +3431,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>549</v>
+      </c>
+      <c r="B20" t="s">
         <v>550</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>551</v>
-      </c>
-      <c r="C20" t="s">
-        <v>552</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
@@ -3454,13 +3451,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B21" t="s">
+        <v>408</v>
+      </c>
+      <c r="C21" t="s">
         <v>409</v>
-      </c>
-      <c r="C21" t="s">
-        <v>410</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
@@ -3474,13 +3471,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B22" t="s">
+        <v>550</v>
+      </c>
+      <c r="C22" t="s">
         <v>551</v>
-      </c>
-      <c r="C22" t="s">
-        <v>552</v>
       </c>
       <c r="D22" t="s">
         <v>3</v>
@@ -3694,7 +3691,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>39</v>
@@ -3834,13 +3831,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>601</v>
+      </c>
+      <c r="B40" t="s">
+        <v>601</v>
+      </c>
+      <c r="C40" t="s">
         <v>602</v>
-      </c>
-      <c r="B40" t="s">
-        <v>602</v>
-      </c>
-      <c r="C40" t="s">
-        <v>603</v>
       </c>
       <c r="D40" t="s">
         <v>3</v>
@@ -4057,10 +4054,10 @@
         <v>14</v>
       </c>
       <c r="B51" t="s">
+        <v>473</v>
+      </c>
+      <c r="C51" t="s">
         <v>474</v>
-      </c>
-      <c r="C51" t="s">
-        <v>475</v>
       </c>
       <c r="D51" t="s">
         <v>3</v>
@@ -4294,7 +4291,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B63" t="s">
         <v>110</v>
@@ -4374,7 +4371,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B67" t="s">
         <v>59</v>
@@ -4574,7 +4571,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -4594,7 +4591,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B78" t="s">
         <v>59</v>
@@ -4614,7 +4611,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B79" t="s">
         <v>132</v>
@@ -4634,7 +4631,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B80" t="s">
         <v>132</v>
@@ -4654,7 +4651,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B81" t="s">
         <v>132</v>
@@ -5554,13 +5551,13 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>608</v>
+      </c>
+      <c r="B126" t="s">
+        <v>608</v>
+      </c>
+      <c r="C126" t="s">
         <v>609</v>
-      </c>
-      <c r="B126" t="s">
-        <v>609</v>
-      </c>
-      <c r="C126" t="s">
-        <v>610</v>
       </c>
       <c r="D126" t="s">
         <v>3</v>
@@ -5594,7 +5591,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B128" t="s">
         <v>235</v>
@@ -5654,7 +5651,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -5797,10 +5794,10 @@
         <v>76</v>
       </c>
       <c r="B138" t="s">
+        <v>523</v>
+      </c>
+      <c r="C138" t="s">
         <v>524</v>
-      </c>
-      <c r="C138" t="s">
-        <v>525</v>
       </c>
       <c r="D138" t="s">
         <v>3</v>
@@ -5814,13 +5811,13 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>610</v>
+      </c>
+      <c r="B139" t="s">
+        <v>610</v>
+      </c>
+      <c r="C139" t="s">
         <v>611</v>
-      </c>
-      <c r="B139" t="s">
-        <v>611</v>
-      </c>
-      <c r="C139" t="s">
-        <v>612</v>
       </c>
       <c r="D139" t="s">
         <v>3</v>
@@ -5834,7 +5831,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B140" t="s">
         <v>239</v>
@@ -5994,10 +5991,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B148" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C148" t="s">
         <v>57</v>
@@ -6040,7 +6037,7 @@
         <v>255</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D150" t="s">
         <v>3</v>
@@ -6334,13 +6331,13 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>614</v>
+      </c>
+      <c r="B165" t="s">
+        <v>614</v>
+      </c>
+      <c r="C165" t="s">
         <v>615</v>
-      </c>
-      <c r="B165" t="s">
-        <v>615</v>
-      </c>
-      <c r="C165" t="s">
-        <v>616</v>
       </c>
       <c r="D165" t="s">
         <v>3</v>
@@ -6640,7 +6637,7 @@
         <v>307</v>
       </c>
       <c r="C180" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D180" t="s">
         <v>3</v>
@@ -6657,7 +6654,7 @@
         <v>308</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C181" t="s">
         <v>309</v>
@@ -6677,7 +6674,7 @@
         <v>310</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C182" t="s">
         <v>311</v>
@@ -6797,10 +6794,10 @@
         <v>136</v>
       </c>
       <c r="B188" t="s">
+        <v>523</v>
+      </c>
+      <c r="C188" t="s">
         <v>524</v>
-      </c>
-      <c r="C188" t="s">
-        <v>525</v>
       </c>
       <c r="D188" t="s">
         <v>3</v>
@@ -6814,7 +6811,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B189" t="s">
         <v>59</v>
@@ -7334,13 +7331,13 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
+        <v>618</v>
+      </c>
+      <c r="B215" t="s">
+        <v>618</v>
+      </c>
+      <c r="C215" t="s">
         <v>619</v>
-      </c>
-      <c r="B215" t="s">
-        <v>619</v>
-      </c>
-      <c r="C215" t="s">
-        <v>620</v>
       </c>
       <c r="D215" t="s">
         <v>3</v>
@@ -7517,16 +7514,16 @@
         <v>380</v>
       </c>
       <c r="B224" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C224" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D224" t="s">
         <v>3</v>
       </c>
       <c r="E224" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="F224" t="s">
         <v>13</v>
@@ -7534,13 +7531,13 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
+        <v>381</v>
+      </c>
+      <c r="B225" t="s">
+        <v>381</v>
+      </c>
+      <c r="C225" t="s">
         <v>382</v>
-      </c>
-      <c r="B225" t="s">
-        <v>382</v>
-      </c>
-      <c r="C225" t="s">
-        <v>383</v>
       </c>
       <c r="D225" t="s">
         <v>3</v>
@@ -7554,13 +7551,13 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
+        <v>383</v>
+      </c>
+      <c r="B226" t="s">
+        <v>383</v>
+      </c>
+      <c r="C226" t="s">
         <v>384</v>
-      </c>
-      <c r="B226" t="s">
-        <v>384</v>
-      </c>
-      <c r="C226" t="s">
-        <v>385</v>
       </c>
       <c r="D226" t="s">
         <v>3</v>
@@ -7574,13 +7571,13 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
+        <v>385</v>
+      </c>
+      <c r="B227" t="s">
+        <v>385</v>
+      </c>
+      <c r="C227" t="s">
         <v>386</v>
-      </c>
-      <c r="B227" t="s">
-        <v>386</v>
-      </c>
-      <c r="C227" t="s">
-        <v>387</v>
       </c>
       <c r="D227" t="s">
         <v>3</v>
@@ -7594,13 +7591,13 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
+        <v>620</v>
+      </c>
+      <c r="B228" t="s">
+        <v>620</v>
+      </c>
+      <c r="C228" t="s">
         <v>621</v>
-      </c>
-      <c r="B228" t="s">
-        <v>621</v>
-      </c>
-      <c r="C228" t="s">
-        <v>622</v>
       </c>
       <c r="D228" t="s">
         <v>3</v>
@@ -7614,13 +7611,13 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
+        <v>387</v>
+      </c>
+      <c r="B229" t="s">
+        <v>387</v>
+      </c>
+      <c r="C229" t="s">
         <v>388</v>
-      </c>
-      <c r="B229" t="s">
-        <v>388</v>
-      </c>
-      <c r="C229" t="s">
-        <v>389</v>
       </c>
       <c r="D229" t="s">
         <v>3</v>
@@ -7634,13 +7631,13 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>389</v>
+      </c>
+      <c r="B230" t="s">
+        <v>389</v>
+      </c>
+      <c r="C230" t="s">
         <v>390</v>
-      </c>
-      <c r="B230" t="s">
-        <v>390</v>
-      </c>
-      <c r="C230" t="s">
-        <v>391</v>
       </c>
       <c r="D230" t="s">
         <v>3</v>
@@ -7654,13 +7651,13 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
+        <v>391</v>
+      </c>
+      <c r="B231" t="s">
+        <v>391</v>
+      </c>
+      <c r="C231" t="s">
         <v>392</v>
-      </c>
-      <c r="B231" t="s">
-        <v>392</v>
-      </c>
-      <c r="C231" t="s">
-        <v>393</v>
       </c>
       <c r="D231" t="s">
         <v>3</v>
@@ -7674,13 +7671,13 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>393</v>
+      </c>
+      <c r="B232" t="s">
+        <v>393</v>
+      </c>
+      <c r="C232" t="s">
         <v>394</v>
-      </c>
-      <c r="B232" t="s">
-        <v>394</v>
-      </c>
-      <c r="C232" t="s">
-        <v>395</v>
       </c>
       <c r="D232" t="s">
         <v>3</v>
@@ -7694,13 +7691,13 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>395</v>
+      </c>
+      <c r="B233" t="s">
+        <v>395</v>
+      </c>
+      <c r="C233" t="s">
         <v>396</v>
-      </c>
-      <c r="B233" t="s">
-        <v>396</v>
-      </c>
-      <c r="C233" t="s">
-        <v>397</v>
       </c>
       <c r="D233" t="s">
         <v>3</v>
@@ -7714,13 +7711,13 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
+        <v>397</v>
+      </c>
+      <c r="B234" t="s">
+        <v>397</v>
+      </c>
+      <c r="C234" t="s">
         <v>398</v>
-      </c>
-      <c r="B234" t="s">
-        <v>398</v>
-      </c>
-      <c r="C234" t="s">
-        <v>399</v>
       </c>
       <c r="D234" t="s">
         <v>3</v>
@@ -7794,13 +7791,13 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
+        <v>622</v>
+      </c>
+      <c r="B238" t="s">
+        <v>622</v>
+      </c>
+      <c r="C238" t="s">
         <v>623</v>
-      </c>
-      <c r="B238" t="s">
-        <v>623</v>
-      </c>
-      <c r="C238" t="s">
-        <v>624</v>
       </c>
       <c r="D238" t="s">
         <v>105</v>
@@ -7814,13 +7811,13 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
+        <v>399</v>
+      </c>
+      <c r="B239" t="s">
+        <v>399</v>
+      </c>
+      <c r="C239" t="s">
         <v>400</v>
-      </c>
-      <c r="B239" t="s">
-        <v>400</v>
-      </c>
-      <c r="C239" t="s">
-        <v>401</v>
       </c>
       <c r="D239" t="s">
         <v>105</v>
@@ -7834,13 +7831,13 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
+        <v>401</v>
+      </c>
+      <c r="B240" t="s">
+        <v>401</v>
+      </c>
+      <c r="C240" t="s">
         <v>402</v>
-      </c>
-      <c r="B240" t="s">
-        <v>402</v>
-      </c>
-      <c r="C240" t="s">
-        <v>403</v>
       </c>
       <c r="D240" t="s">
         <v>3</v>
@@ -7854,13 +7851,13 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
+        <v>403</v>
+      </c>
+      <c r="B241" t="s">
+        <v>403</v>
+      </c>
+      <c r="C241" t="s">
         <v>404</v>
-      </c>
-      <c r="B241" t="s">
-        <v>404</v>
-      </c>
-      <c r="C241" t="s">
-        <v>405</v>
       </c>
       <c r="D241" t="s">
         <v>3</v>
@@ -7874,13 +7871,13 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
+        <v>405</v>
+      </c>
+      <c r="B242" t="s">
+        <v>405</v>
+      </c>
+      <c r="C242" t="s">
         <v>406</v>
-      </c>
-      <c r="B242" t="s">
-        <v>406</v>
-      </c>
-      <c r="C242" t="s">
-        <v>407</v>
       </c>
       <c r="D242" t="s">
         <v>105</v>
@@ -7894,13 +7891,13 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
+        <v>407</v>
+      </c>
+      <c r="B243" t="s">
         <v>408</v>
       </c>
-      <c r="B243" t="s">
+      <c r="C243" t="s">
         <v>409</v>
-      </c>
-      <c r="C243" t="s">
-        <v>410</v>
       </c>
       <c r="D243" t="s">
         <v>3</v>
@@ -7914,13 +7911,13 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B244" t="s">
+        <v>408</v>
+      </c>
+      <c r="C244" t="s">
         <v>409</v>
-      </c>
-      <c r="C244" t="s">
-        <v>410</v>
       </c>
       <c r="D244" t="s">
         <v>3</v>
@@ -7934,13 +7931,13 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B245" t="s">
+        <v>408</v>
+      </c>
+      <c r="C245" t="s">
         <v>409</v>
-      </c>
-      <c r="C245" t="s">
-        <v>410</v>
       </c>
       <c r="D245" t="s">
         <v>3</v>
@@ -7954,13 +7951,13 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
+        <v>408</v>
+      </c>
+      <c r="B246" t="s">
+        <v>408</v>
+      </c>
+      <c r="C246" t="s">
         <v>409</v>
-      </c>
-      <c r="B246" t="s">
-        <v>409</v>
-      </c>
-      <c r="C246" t="s">
-        <v>410</v>
       </c>
       <c r="D246" t="s">
         <v>3</v>
@@ -7974,13 +7971,13 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
+        <v>411</v>
+      </c>
+      <c r="B247" t="s">
+        <v>411</v>
+      </c>
+      <c r="C247" t="s">
         <v>412</v>
-      </c>
-      <c r="B247" t="s">
-        <v>412</v>
-      </c>
-      <c r="C247" t="s">
-        <v>413</v>
       </c>
       <c r="D247" t="s">
         <v>3</v>
@@ -7994,13 +7991,13 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
+        <v>413</v>
+      </c>
+      <c r="B248" t="s">
+        <v>413</v>
+      </c>
+      <c r="C248" t="s">
         <v>414</v>
-      </c>
-      <c r="B248" t="s">
-        <v>414</v>
-      </c>
-      <c r="C248" t="s">
-        <v>415</v>
       </c>
       <c r="D248" t="s">
         <v>105</v>
@@ -8014,13 +8011,13 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
+        <v>415</v>
+      </c>
+      <c r="B249" t="s">
+        <v>415</v>
+      </c>
+      <c r="C249" t="s">
         <v>416</v>
-      </c>
-      <c r="B249" t="s">
-        <v>416</v>
-      </c>
-      <c r="C249" t="s">
-        <v>417</v>
       </c>
       <c r="D249" t="s">
         <v>3</v>
@@ -8034,13 +8031,13 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
+        <v>417</v>
+      </c>
+      <c r="B250" t="s">
+        <v>417</v>
+      </c>
+      <c r="C250" t="s">
         <v>418</v>
-      </c>
-      <c r="B250" t="s">
-        <v>418</v>
-      </c>
-      <c r="C250" t="s">
-        <v>419</v>
       </c>
       <c r="D250" t="s">
         <v>105</v>
@@ -8054,13 +8051,13 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
+        <v>419</v>
+      </c>
+      <c r="B251" t="s">
+        <v>419</v>
+      </c>
+      <c r="C251" t="s">
         <v>420</v>
-      </c>
-      <c r="B251" t="s">
-        <v>420</v>
-      </c>
-      <c r="C251" t="s">
-        <v>421</v>
       </c>
       <c r="D251" t="s">
         <v>3</v>
@@ -8074,13 +8071,13 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
+        <v>421</v>
+      </c>
+      <c r="B252" t="s">
+        <v>421</v>
+      </c>
+      <c r="C252" t="s">
         <v>422</v>
-      </c>
-      <c r="B252" t="s">
-        <v>422</v>
-      </c>
-      <c r="C252" t="s">
-        <v>423</v>
       </c>
       <c r="D252" t="s">
         <v>3</v>
@@ -8094,13 +8091,13 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
+        <v>423</v>
+      </c>
+      <c r="B253" t="s">
+        <v>423</v>
+      </c>
+      <c r="C253" t="s">
         <v>424</v>
-      </c>
-      <c r="B253" t="s">
-        <v>424</v>
-      </c>
-      <c r="C253" t="s">
-        <v>425</v>
       </c>
       <c r="D253" t="s">
         <v>105</v>
@@ -8114,13 +8111,13 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
+        <v>425</v>
+      </c>
+      <c r="B254" t="s">
+        <v>425</v>
+      </c>
+      <c r="C254" t="s">
         <v>426</v>
-      </c>
-      <c r="B254" t="s">
-        <v>426</v>
-      </c>
-      <c r="C254" t="s">
-        <v>427</v>
       </c>
       <c r="D254" t="s">
         <v>3</v>
@@ -8134,13 +8131,13 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
+        <v>427</v>
+      </c>
+      <c r="B255" t="s">
+        <v>427</v>
+      </c>
+      <c r="C255" t="s">
         <v>428</v>
-      </c>
-      <c r="B255" t="s">
-        <v>428</v>
-      </c>
-      <c r="C255" t="s">
-        <v>429</v>
       </c>
       <c r="D255" t="s">
         <v>3</v>
@@ -8154,13 +8151,13 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
+        <v>429</v>
+      </c>
+      <c r="B256" t="s">
+        <v>429</v>
+      </c>
+      <c r="C256" t="s">
         <v>430</v>
-      </c>
-      <c r="B256" t="s">
-        <v>430</v>
-      </c>
-      <c r="C256" t="s">
-        <v>431</v>
       </c>
       <c r="D256" t="s">
         <v>3</v>
@@ -8257,10 +8254,10 @@
         <v>18</v>
       </c>
       <c r="B261" t="s">
+        <v>523</v>
+      </c>
+      <c r="C261" t="s">
         <v>524</v>
-      </c>
-      <c r="C261" t="s">
-        <v>525</v>
       </c>
       <c r="D261" t="s">
         <v>3</v>
@@ -8357,10 +8354,10 @@
         <v>78</v>
       </c>
       <c r="B266" t="s">
+        <v>523</v>
+      </c>
+      <c r="C266" t="s">
         <v>524</v>
-      </c>
-      <c r="C266" t="s">
-        <v>525</v>
       </c>
       <c r="D266" t="s">
         <v>3</v>
@@ -8374,13 +8371,13 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B267" t="s">
+        <v>488</v>
+      </c>
+      <c r="C267" t="s">
         <v>489</v>
-      </c>
-      <c r="C267" t="s">
-        <v>490</v>
       </c>
       <c r="D267" t="s">
         <v>3</v>
@@ -8434,7 +8431,7 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B270" t="s">
         <v>59</v>
@@ -8454,7 +8451,7 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B271" t="s">
         <v>120</v>
@@ -8474,7 +8471,7 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B272" t="s">
         <v>132</v>
@@ -8537,10 +8534,10 @@
         <v>19</v>
       </c>
       <c r="B275" t="s">
+        <v>523</v>
+      </c>
+      <c r="C275" t="s">
         <v>524</v>
-      </c>
-      <c r="C275" t="s">
-        <v>525</v>
       </c>
       <c r="D275" t="s">
         <v>3</v>
@@ -8594,7 +8591,7 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B278" t="s">
         <v>59</v>
@@ -8614,7 +8611,7 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B279" t="s">
         <v>132</v>
@@ -8634,7 +8631,7 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B280" t="s">
         <v>132</v>
@@ -8694,7 +8691,7 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B283" t="s">
         <v>59</v>
@@ -8754,7 +8751,7 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B286" t="s">
         <v>59</v>
@@ -8774,7 +8771,7 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B287" t="s">
         <v>59</v>
@@ -8794,7 +8791,7 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B288" t="s">
         <v>277</v>
@@ -8814,13 +8811,13 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B289" t="s">
+        <v>523</v>
+      </c>
+      <c r="C289" t="s">
         <v>524</v>
-      </c>
-      <c r="C289" t="s">
-        <v>525</v>
       </c>
       <c r="D289" t="s">
         <v>3</v>
@@ -8834,7 +8831,7 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B290" t="s">
         <v>59</v>
@@ -8854,7 +8851,7 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B291" t="s">
         <v>132</v>
@@ -8917,10 +8914,10 @@
         <v>82</v>
       </c>
       <c r="B294" t="s">
+        <v>523</v>
+      </c>
+      <c r="C294" t="s">
         <v>524</v>
-      </c>
-      <c r="C294" t="s">
-        <v>525</v>
       </c>
       <c r="D294" t="s">
         <v>3</v>
@@ -8934,7 +8931,7 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B295" t="s">
         <v>59</v>
@@ -8954,7 +8951,7 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B296" t="s">
         <v>132</v>
@@ -8974,13 +8971,13 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B297" t="s">
+        <v>473</v>
+      </c>
+      <c r="C297" t="s">
         <v>474</v>
-      </c>
-      <c r="C297" t="s">
-        <v>475</v>
       </c>
       <c r="D297" t="s">
         <v>3</v>
@@ -8994,7 +8991,7 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B298" t="s">
         <v>59</v>
@@ -9014,7 +9011,7 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B299" t="s">
         <v>132</v>
@@ -9034,7 +9031,7 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B300" t="s">
         <v>15</v>
@@ -9054,7 +9051,7 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B301" t="s">
         <v>59</v>
@@ -9074,7 +9071,7 @@
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B302" t="s">
         <v>59</v>
@@ -9094,7 +9091,7 @@
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B303" t="s">
         <v>132</v>
@@ -9154,7 +9151,7 @@
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B306" t="s">
         <v>59</v>
@@ -9174,7 +9171,7 @@
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B307" t="s">
         <v>132</v>
@@ -9257,10 +9254,10 @@
         <v>84</v>
       </c>
       <c r="B311" t="s">
+        <v>473</v>
+      </c>
+      <c r="C311" t="s">
         <v>474</v>
-      </c>
-      <c r="C311" t="s">
-        <v>475</v>
       </c>
       <c r="D311" t="s">
         <v>3</v>
@@ -9277,10 +9274,10 @@
         <v>84</v>
       </c>
       <c r="B312" t="s">
+        <v>523</v>
+      </c>
+      <c r="C312" t="s">
         <v>524</v>
-      </c>
-      <c r="C312" t="s">
-        <v>525</v>
       </c>
       <c r="D312" t="s">
         <v>3</v>
@@ -9294,13 +9291,13 @@
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
+        <v>431</v>
+      </c>
+      <c r="B313" t="s">
+        <v>431</v>
+      </c>
+      <c r="C313" t="s">
         <v>432</v>
-      </c>
-      <c r="B313" t="s">
-        <v>432</v>
-      </c>
-      <c r="C313" t="s">
-        <v>433</v>
       </c>
       <c r="D313" t="s">
         <v>3</v>
@@ -9314,7 +9311,7 @@
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B314" t="s">
         <v>120</v>
@@ -9334,7 +9331,7 @@
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B315" t="s">
         <v>15</v>
@@ -9354,7 +9351,7 @@
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B316" t="s">
         <v>59</v>
@@ -9374,7 +9371,7 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B317" t="s">
         <v>120</v>
@@ -9394,13 +9391,13 @@
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B318" t="s">
+        <v>523</v>
+      </c>
+      <c r="C318" t="s">
         <v>524</v>
-      </c>
-      <c r="C318" t="s">
-        <v>525</v>
       </c>
       <c r="D318" t="s">
         <v>3</v>
@@ -9434,13 +9431,13 @@
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B320" t="s">
+        <v>523</v>
+      </c>
+      <c r="C320" t="s">
         <v>524</v>
-      </c>
-      <c r="C320" t="s">
-        <v>525</v>
       </c>
       <c r="D320" t="s">
         <v>3</v>
@@ -9474,13 +9471,13 @@
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
+        <v>433</v>
+      </c>
+      <c r="B322" t="s">
+        <v>433</v>
+      </c>
+      <c r="C322" t="s">
         <v>434</v>
-      </c>
-      <c r="B322" t="s">
-        <v>434</v>
-      </c>
-      <c r="C322" t="s">
-        <v>435</v>
       </c>
       <c r="D322" t="s">
         <v>105</v>
@@ -9494,13 +9491,13 @@
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
+        <v>435</v>
+      </c>
+      <c r="B323" t="s">
+        <v>435</v>
+      </c>
+      <c r="C323" t="s">
         <v>436</v>
-      </c>
-      <c r="B323" t="s">
-        <v>436</v>
-      </c>
-      <c r="C323" t="s">
-        <v>437</v>
       </c>
       <c r="D323" t="s">
         <v>3</v>
@@ -9514,13 +9511,13 @@
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
+        <v>437</v>
+      </c>
+      <c r="B324" t="s">
+        <v>437</v>
+      </c>
+      <c r="C324" t="s">
         <v>438</v>
-      </c>
-      <c r="B324" t="s">
-        <v>438</v>
-      </c>
-      <c r="C324" t="s">
-        <v>439</v>
       </c>
       <c r="D324" t="s">
         <v>3</v>
@@ -9534,13 +9531,13 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
+        <v>439</v>
+      </c>
+      <c r="B325" t="s">
+        <v>439</v>
+      </c>
+      <c r="C325" t="s">
         <v>440</v>
-      </c>
-      <c r="B325" t="s">
-        <v>440</v>
-      </c>
-      <c r="C325" t="s">
-        <v>441</v>
       </c>
       <c r="D325" t="s">
         <v>105</v>
@@ -9554,13 +9551,13 @@
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
+        <v>441</v>
+      </c>
+      <c r="B326" t="s">
+        <v>441</v>
+      </c>
+      <c r="C326" t="s">
         <v>442</v>
-      </c>
-      <c r="B326" t="s">
-        <v>442</v>
-      </c>
-      <c r="C326" t="s">
-        <v>443</v>
       </c>
       <c r="D326" t="s">
         <v>3</v>
@@ -9574,13 +9571,13 @@
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
+        <v>444</v>
+      </c>
+      <c r="B327" t="s">
+        <v>444</v>
+      </c>
+      <c r="C327" t="s">
         <v>445</v>
-      </c>
-      <c r="B327" t="s">
-        <v>445</v>
-      </c>
-      <c r="C327" t="s">
-        <v>446</v>
       </c>
       <c r="D327" t="s">
         <v>3</v>
@@ -9594,13 +9591,13 @@
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
+        <v>443</v>
+      </c>
+      <c r="B328" t="s">
         <v>444</v>
       </c>
-      <c r="B328" t="s">
+      <c r="C328" t="s">
         <v>445</v>
-      </c>
-      <c r="C328" t="s">
-        <v>446</v>
       </c>
       <c r="D328" t="s">
         <v>3</v>
@@ -9614,13 +9611,13 @@
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
+        <v>447</v>
+      </c>
+      <c r="B329" t="s">
+        <v>447</v>
+      </c>
+      <c r="C329" t="s">
         <v>448</v>
-      </c>
-      <c r="B329" t="s">
-        <v>448</v>
-      </c>
-      <c r="C329" t="s">
-        <v>449</v>
       </c>
       <c r="D329" t="s">
         <v>3</v>
@@ -9634,13 +9631,13 @@
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
+        <v>449</v>
+      </c>
+      <c r="B330" t="s">
+        <v>449</v>
+      </c>
+      <c r="C330" t="s">
         <v>450</v>
-      </c>
-      <c r="B330" t="s">
-        <v>450</v>
-      </c>
-      <c r="C330" t="s">
-        <v>451</v>
       </c>
       <c r="D330" t="s">
         <v>3</v>
@@ -9654,13 +9651,13 @@
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B331" t="s">
+        <v>453</v>
+      </c>
+      <c r="C331" t="s">
         <v>454</v>
-      </c>
-      <c r="C331" t="s">
-        <v>455</v>
       </c>
       <c r="D331" t="s">
         <v>3</v>
@@ -9674,13 +9671,13 @@
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
+        <v>451</v>
+      </c>
+      <c r="B332" t="s">
+        <v>451</v>
+      </c>
+      <c r="C332" t="s">
         <v>452</v>
-      </c>
-      <c r="B332" t="s">
-        <v>452</v>
-      </c>
-      <c r="C332" t="s">
-        <v>453</v>
       </c>
       <c r="D332" t="s">
         <v>3</v>
@@ -9694,13 +9691,13 @@
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
+        <v>453</v>
+      </c>
+      <c r="B333" t="s">
+        <v>453</v>
+      </c>
+      <c r="C333" t="s">
         <v>454</v>
-      </c>
-      <c r="B333" t="s">
-        <v>454</v>
-      </c>
-      <c r="C333" t="s">
-        <v>455</v>
       </c>
       <c r="D333" t="s">
         <v>3</v>
@@ -9714,13 +9711,13 @@
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
+        <v>640</v>
+      </c>
+      <c r="B334" t="s">
+        <v>640</v>
+      </c>
+      <c r="C334" t="s">
         <v>641</v>
-      </c>
-      <c r="B334" t="s">
-        <v>641</v>
-      </c>
-      <c r="C334" t="s">
-        <v>642</v>
       </c>
       <c r="D334" t="s">
         <v>3</v>
@@ -9734,13 +9731,13 @@
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
+        <v>455</v>
+      </c>
+      <c r="B335" t="s">
+        <v>455</v>
+      </c>
+      <c r="C335" t="s">
         <v>456</v>
-      </c>
-      <c r="B335" t="s">
-        <v>456</v>
-      </c>
-      <c r="C335" t="s">
-        <v>457</v>
       </c>
       <c r="D335" t="s">
         <v>3</v>
@@ -9754,13 +9751,13 @@
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
+        <v>457</v>
+      </c>
+      <c r="B336" t="s">
+        <v>457</v>
+      </c>
+      <c r="C336" t="s">
         <v>458</v>
-      </c>
-      <c r="B336" t="s">
-        <v>458</v>
-      </c>
-      <c r="C336" t="s">
-        <v>459</v>
       </c>
       <c r="D336" t="s">
         <v>3</v>
@@ -9774,13 +9771,13 @@
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
+        <v>459</v>
+      </c>
+      <c r="B337" t="s">
+        <v>459</v>
+      </c>
+      <c r="C337" t="s">
         <v>460</v>
-      </c>
-      <c r="B337" t="s">
-        <v>460</v>
-      </c>
-      <c r="C337" t="s">
-        <v>461</v>
       </c>
       <c r="D337" t="s">
         <v>3</v>
@@ -9794,13 +9791,13 @@
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
+        <v>461</v>
+      </c>
+      <c r="B338" t="s">
+        <v>461</v>
+      </c>
+      <c r="C338" t="s">
         <v>462</v>
-      </c>
-      <c r="B338" t="s">
-        <v>462</v>
-      </c>
-      <c r="C338" t="s">
-        <v>463</v>
       </c>
       <c r="D338" t="s">
         <v>3</v>
@@ -9814,13 +9811,13 @@
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
+        <v>463</v>
+      </c>
+      <c r="B339" t="s">
+        <v>463</v>
+      </c>
+      <c r="C339" t="s">
         <v>464</v>
-      </c>
-      <c r="B339" t="s">
-        <v>464</v>
-      </c>
-      <c r="C339" t="s">
-        <v>465</v>
       </c>
       <c r="D339" t="s">
         <v>3</v>
@@ -9834,13 +9831,13 @@
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
+        <v>465</v>
+      </c>
+      <c r="B340" t="s">
+        <v>465</v>
+      </c>
+      <c r="C340" t="s">
         <v>466</v>
-      </c>
-      <c r="B340" t="s">
-        <v>466</v>
-      </c>
-      <c r="C340" t="s">
-        <v>467</v>
       </c>
       <c r="D340" t="s">
         <v>25</v>
@@ -9854,13 +9851,13 @@
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
+        <v>467</v>
+      </c>
+      <c r="B341" t="s">
+        <v>467</v>
+      </c>
+      <c r="C341" t="s">
         <v>468</v>
-      </c>
-      <c r="B341" t="s">
-        <v>468</v>
-      </c>
-      <c r="C341" t="s">
-        <v>469</v>
       </c>
       <c r="D341" t="s">
         <v>25</v>
@@ -9874,13 +9871,13 @@
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
+        <v>469</v>
+      </c>
+      <c r="B342" t="s">
+        <v>469</v>
+      </c>
+      <c r="C342" t="s">
         <v>470</v>
-      </c>
-      <c r="B342" t="s">
-        <v>470</v>
-      </c>
-      <c r="C342" t="s">
-        <v>471</v>
       </c>
       <c r="D342" t="s">
         <v>3</v>
@@ -9894,13 +9891,13 @@
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
+        <v>471</v>
+      </c>
+      <c r="B343" t="s">
+        <v>471</v>
+      </c>
+      <c r="C343" t="s">
         <v>472</v>
-      </c>
-      <c r="B343" t="s">
-        <v>472</v>
-      </c>
-      <c r="C343" t="s">
-        <v>473</v>
       </c>
       <c r="D343" t="s">
         <v>3</v>
@@ -9914,13 +9911,13 @@
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
+        <v>473</v>
+      </c>
+      <c r="B344" t="s">
+        <v>473</v>
+      </c>
+      <c r="C344" t="s">
         <v>474</v>
-      </c>
-      <c r="B344" t="s">
-        <v>474</v>
-      </c>
-      <c r="C344" t="s">
-        <v>475</v>
       </c>
       <c r="D344" t="s">
         <v>3</v>
@@ -9934,13 +9931,13 @@
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
+        <v>475</v>
+      </c>
+      <c r="B345" t="s">
+        <v>475</v>
+      </c>
+      <c r="C345" t="s">
         <v>476</v>
-      </c>
-      <c r="B345" t="s">
-        <v>476</v>
-      </c>
-      <c r="C345" t="s">
-        <v>477</v>
       </c>
       <c r="D345" t="s">
         <v>3</v>
@@ -9954,13 +9951,13 @@
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
+        <v>477</v>
+      </c>
+      <c r="B346" t="s">
+        <v>477</v>
+      </c>
+      <c r="C346" t="s">
         <v>478</v>
-      </c>
-      <c r="B346" t="s">
-        <v>478</v>
-      </c>
-      <c r="C346" t="s">
-        <v>479</v>
       </c>
       <c r="D346" t="s">
         <v>3</v>
@@ -9974,13 +9971,13 @@
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
+        <v>479</v>
+      </c>
+      <c r="B347" t="s">
+        <v>479</v>
+      </c>
+      <c r="C347" t="s">
         <v>480</v>
-      </c>
-      <c r="B347" t="s">
-        <v>480</v>
-      </c>
-      <c r="C347" t="s">
-        <v>481</v>
       </c>
       <c r="D347" t="s">
         <v>3</v>
@@ -9994,13 +9991,13 @@
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
+        <v>481</v>
+      </c>
+      <c r="B348" t="s">
+        <v>481</v>
+      </c>
+      <c r="C348" t="s">
         <v>482</v>
-      </c>
-      <c r="B348" t="s">
-        <v>482</v>
-      </c>
-      <c r="C348" t="s">
-        <v>483</v>
       </c>
       <c r="D348" t="s">
         <v>3</v>
@@ -10014,13 +10011,13 @@
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
+        <v>483</v>
+      </c>
+      <c r="B349" t="s">
+        <v>483</v>
+      </c>
+      <c r="C349" t="s">
         <v>484</v>
-      </c>
-      <c r="B349" t="s">
-        <v>484</v>
-      </c>
-      <c r="C349" t="s">
-        <v>485</v>
       </c>
       <c r="D349" t="s">
         <v>25</v>
@@ -10034,13 +10031,13 @@
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
+        <v>485</v>
+      </c>
+      <c r="B350" t="s">
+        <v>485</v>
+      </c>
+      <c r="C350" t="s">
         <v>486</v>
-      </c>
-      <c r="B350" t="s">
-        <v>486</v>
-      </c>
-      <c r="C350" t="s">
-        <v>487</v>
       </c>
       <c r="D350" t="s">
         <v>3</v>
@@ -10054,13 +10051,13 @@
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
+        <v>488</v>
+      </c>
+      <c r="B351" t="s">
+        <v>488</v>
+      </c>
+      <c r="C351" t="s">
         <v>489</v>
-      </c>
-      <c r="B351" t="s">
-        <v>489</v>
-      </c>
-      <c r="C351" t="s">
-        <v>490</v>
       </c>
       <c r="D351" t="s">
         <v>3</v>
@@ -10074,13 +10071,13 @@
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
+        <v>492</v>
+      </c>
+      <c r="B352" t="s">
+        <v>492</v>
+      </c>
+      <c r="C352" t="s">
         <v>493</v>
-      </c>
-      <c r="B352" t="s">
-        <v>493</v>
-      </c>
-      <c r="C352" t="s">
-        <v>494</v>
       </c>
       <c r="D352" t="s">
         <v>3</v>
@@ -10094,13 +10091,13 @@
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
+        <v>494</v>
+      </c>
+      <c r="B353" t="s">
+        <v>494</v>
+      </c>
+      <c r="C353" t="s">
         <v>495</v>
-      </c>
-      <c r="B353" t="s">
-        <v>495</v>
-      </c>
-      <c r="C353" t="s">
-        <v>496</v>
       </c>
       <c r="D353" t="s">
         <v>3</v>
@@ -10114,13 +10111,13 @@
     </row>
     <row r="354" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
+        <v>496</v>
+      </c>
+      <c r="B354" t="s">
+        <v>496</v>
+      </c>
+      <c r="C354" t="s">
         <v>497</v>
-      </c>
-      <c r="B354" t="s">
-        <v>497</v>
-      </c>
-      <c r="C354" t="s">
-        <v>498</v>
       </c>
       <c r="D354" t="s">
         <v>3</v>
@@ -10134,13 +10131,13 @@
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
+        <v>498</v>
+      </c>
+      <c r="B355" t="s">
+        <v>498</v>
+      </c>
+      <c r="C355" t="s">
         <v>499</v>
-      </c>
-      <c r="B355" t="s">
-        <v>499</v>
-      </c>
-      <c r="C355" t="s">
-        <v>500</v>
       </c>
       <c r="D355" t="s">
         <v>3</v>
@@ -10154,13 +10151,13 @@
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
+        <v>501</v>
+      </c>
+      <c r="B356" t="s">
+        <v>501</v>
+      </c>
+      <c r="C356" t="s">
         <v>502</v>
-      </c>
-      <c r="B356" t="s">
-        <v>502</v>
-      </c>
-      <c r="C356" t="s">
-        <v>503</v>
       </c>
       <c r="D356" t="s">
         <v>3</v>
@@ -10174,13 +10171,13 @@
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
+        <v>500</v>
+      </c>
+      <c r="B357" t="s">
         <v>501</v>
       </c>
-      <c r="B357" t="s">
+      <c r="C357" t="s">
         <v>502</v>
-      </c>
-      <c r="C357" t="s">
-        <v>503</v>
       </c>
       <c r="D357" t="s">
         <v>3</v>
@@ -10194,7 +10191,7 @@
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B358">
         <v>0</v>
@@ -10277,10 +10274,10 @@
         <v>85</v>
       </c>
       <c r="B362" t="s">
+        <v>523</v>
+      </c>
+      <c r="C362" t="s">
         <v>524</v>
-      </c>
-      <c r="C362" t="s">
-        <v>525</v>
       </c>
       <c r="D362" t="s">
         <v>3</v>
@@ -10314,13 +10311,13 @@
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B364" t="s">
+        <v>408</v>
+      </c>
+      <c r="C364" t="s">
         <v>409</v>
-      </c>
-      <c r="C364" t="s">
-        <v>410</v>
       </c>
       <c r="D364" t="s">
         <v>3</v>
@@ -10334,13 +10331,13 @@
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B365" t="s">
+        <v>408</v>
+      </c>
+      <c r="C365" t="s">
         <v>409</v>
-      </c>
-      <c r="C365" t="s">
-        <v>410</v>
       </c>
       <c r="D365" t="s">
         <v>3</v>
@@ -10354,13 +10351,13 @@
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B366" t="s">
+        <v>550</v>
+      </c>
+      <c r="C366" t="s">
         <v>551</v>
-      </c>
-      <c r="C366" t="s">
-        <v>552</v>
       </c>
       <c r="D366" t="s">
         <v>3</v>
@@ -10394,13 +10391,13 @@
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B368" t="s">
+        <v>444</v>
+      </c>
+      <c r="C368" t="s">
         <v>445</v>
-      </c>
-      <c r="C368" t="s">
-        <v>446</v>
       </c>
       <c r="D368" t="s">
         <v>3</v>
@@ -10414,13 +10411,13 @@
     </row>
     <row r="369" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B369" t="s">
+        <v>453</v>
+      </c>
+      <c r="C369" t="s">
         <v>454</v>
-      </c>
-      <c r="C369" t="s">
-        <v>455</v>
       </c>
       <c r="D369" t="s">
         <v>3</v>
@@ -10434,13 +10431,13 @@
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B370" t="s">
+        <v>550</v>
+      </c>
+      <c r="C370" t="s">
         <v>551</v>
-      </c>
-      <c r="C370" t="s">
-        <v>552</v>
       </c>
       <c r="D370" t="s">
         <v>3</v>
@@ -10477,10 +10474,10 @@
         <v>159</v>
       </c>
       <c r="B372" t="s">
+        <v>550</v>
+      </c>
+      <c r="C372" t="s">
         <v>551</v>
-      </c>
-      <c r="C372" t="s">
-        <v>552</v>
       </c>
       <c r="D372" t="s">
         <v>3</v>
@@ -10557,10 +10554,10 @@
         <v>86</v>
       </c>
       <c r="B376" t="s">
+        <v>523</v>
+      </c>
+      <c r="C376" t="s">
         <v>524</v>
-      </c>
-      <c r="C376" t="s">
-        <v>525</v>
       </c>
       <c r="D376" t="s">
         <v>3</v>
@@ -10574,13 +10571,13 @@
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B377" t="s">
+        <v>488</v>
+      </c>
+      <c r="C377" t="s">
         <v>489</v>
-      </c>
-      <c r="C377" t="s">
-        <v>490</v>
       </c>
       <c r="D377" t="s">
         <v>3</v>
@@ -10594,13 +10591,13 @@
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B378" t="s">
+        <v>550</v>
+      </c>
+      <c r="C378" t="s">
         <v>551</v>
-      </c>
-      <c r="C378" t="s">
-        <v>552</v>
       </c>
       <c r="D378" t="s">
         <v>3</v>
@@ -10657,10 +10654,10 @@
         <v>87</v>
       </c>
       <c r="B381" t="s">
+        <v>523</v>
+      </c>
+      <c r="C381" t="s">
         <v>524</v>
-      </c>
-      <c r="C381" t="s">
-        <v>525</v>
       </c>
       <c r="D381" t="s">
         <v>3</v>
@@ -10714,13 +10711,13 @@
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B384" t="s">
+        <v>550</v>
+      </c>
+      <c r="C384" t="s">
         <v>551</v>
-      </c>
-      <c r="C384" t="s">
-        <v>552</v>
       </c>
       <c r="D384" t="s">
         <v>3</v>
@@ -10734,13 +10731,13 @@
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B385" t="s">
+        <v>408</v>
+      </c>
+      <c r="C385" t="s">
         <v>409</v>
-      </c>
-      <c r="C385" t="s">
-        <v>410</v>
       </c>
       <c r="D385" t="s">
         <v>3</v>
@@ -10754,13 +10751,13 @@
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B386" t="s">
+        <v>550</v>
+      </c>
+      <c r="C386" t="s">
         <v>551</v>
-      </c>
-      <c r="C386" t="s">
-        <v>552</v>
       </c>
       <c r="D386" t="s">
         <v>3</v>
@@ -10774,13 +10771,13 @@
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B387" t="s">
+        <v>550</v>
+      </c>
+      <c r="C387" t="s">
         <v>551</v>
-      </c>
-      <c r="C387" t="s">
-        <v>552</v>
       </c>
       <c r="D387" t="s">
         <v>3</v>
@@ -10794,13 +10791,13 @@
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B388" t="s">
+        <v>550</v>
+      </c>
+      <c r="C388" t="s">
         <v>551</v>
-      </c>
-      <c r="C388" t="s">
-        <v>552</v>
       </c>
       <c r="D388" t="s">
         <v>3</v>
@@ -10857,10 +10854,10 @@
         <v>160</v>
       </c>
       <c r="B391" t="s">
+        <v>488</v>
+      </c>
+      <c r="C391" t="s">
         <v>489</v>
-      </c>
-      <c r="C391" t="s">
-        <v>490</v>
       </c>
       <c r="D391" t="s">
         <v>3</v>
@@ -10877,10 +10874,10 @@
         <v>160</v>
       </c>
       <c r="B392" t="s">
+        <v>550</v>
+      </c>
+      <c r="C392" t="s">
         <v>551</v>
-      </c>
-      <c r="C392" t="s">
-        <v>552</v>
       </c>
       <c r="D392" t="s">
         <v>3</v>
@@ -10894,13 +10891,13 @@
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B393" t="s">
+        <v>550</v>
+      </c>
+      <c r="C393" t="s">
         <v>551</v>
-      </c>
-      <c r="C393" t="s">
-        <v>552</v>
       </c>
       <c r="D393" t="s">
         <v>3</v>
@@ -10994,13 +10991,13 @@
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
+        <v>555</v>
+      </c>
+      <c r="B398" t="s">
         <v>556</v>
       </c>
-      <c r="B398" t="s">
+      <c r="C398" t="s">
         <v>557</v>
-      </c>
-      <c r="C398" t="s">
-        <v>558</v>
       </c>
       <c r="D398" t="s">
         <v>3</v>
@@ -11014,7 +11011,7 @@
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B399" t="s">
         <v>326</v>
@@ -11034,13 +11031,13 @@
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B400" t="s">
+        <v>444</v>
+      </c>
+      <c r="C400" t="s">
         <v>445</v>
-      </c>
-      <c r="C400" t="s">
-        <v>446</v>
       </c>
       <c r="D400" t="s">
         <v>3</v>
@@ -11054,13 +11051,13 @@
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
+        <v>503</v>
+      </c>
+      <c r="B401" t="s">
+        <v>503</v>
+      </c>
+      <c r="C401" t="s">
         <v>504</v>
-      </c>
-      <c r="B401" t="s">
-        <v>504</v>
-      </c>
-      <c r="C401" t="s">
-        <v>505</v>
       </c>
       <c r="D401" t="s">
         <v>3</v>
@@ -11074,13 +11071,13 @@
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
+        <v>505</v>
+      </c>
+      <c r="B402" t="s">
+        <v>505</v>
+      </c>
+      <c r="C402" t="s">
         <v>506</v>
-      </c>
-      <c r="B402" t="s">
-        <v>506</v>
-      </c>
-      <c r="C402" t="s">
-        <v>507</v>
       </c>
       <c r="D402" t="s">
         <v>3</v>
@@ -11094,13 +11091,13 @@
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
+        <v>507</v>
+      </c>
+      <c r="B403" t="s">
         <v>508</v>
       </c>
-      <c r="B403" t="s">
+      <c r="C403" t="s">
         <v>509</v>
-      </c>
-      <c r="C403" t="s">
-        <v>510</v>
       </c>
       <c r="D403" t="s">
         <v>3</v>
@@ -11114,13 +11111,13 @@
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
+        <v>508</v>
+      </c>
+      <c r="B404" t="s">
+        <v>508</v>
+      </c>
+      <c r="C404" t="s">
         <v>509</v>
-      </c>
-      <c r="B404" t="s">
-        <v>509</v>
-      </c>
-      <c r="C404" t="s">
-        <v>510</v>
       </c>
       <c r="D404" t="s">
         <v>3</v>
@@ -11134,13 +11131,13 @@
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
+        <v>510</v>
+      </c>
+      <c r="B405" t="s">
         <v>511</v>
       </c>
-      <c r="B405" t="s">
+      <c r="C405" t="s">
         <v>512</v>
-      </c>
-      <c r="C405" t="s">
-        <v>513</v>
       </c>
       <c r="D405" t="s">
         <v>105</v>
@@ -11154,13 +11151,13 @@
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
+        <v>511</v>
+      </c>
+      <c r="B406" t="s">
+        <v>511</v>
+      </c>
+      <c r="C406" t="s">
         <v>512</v>
-      </c>
-      <c r="B406" t="s">
-        <v>512</v>
-      </c>
-      <c r="C406" t="s">
-        <v>513</v>
       </c>
       <c r="D406" t="s">
         <v>105</v>
@@ -11174,13 +11171,13 @@
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
+        <v>513</v>
+      </c>
+      <c r="B407" t="s">
+        <v>513</v>
+      </c>
+      <c r="C407" t="s">
         <v>514</v>
-      </c>
-      <c r="B407" t="s">
-        <v>514</v>
-      </c>
-      <c r="C407" t="s">
-        <v>515</v>
       </c>
       <c r="D407" t="s">
         <v>105</v>
@@ -11194,13 +11191,13 @@
     </row>
     <row r="408" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
+        <v>515</v>
+      </c>
+      <c r="B408" t="s">
+        <v>515</v>
+      </c>
+      <c r="C408" t="s">
         <v>516</v>
-      </c>
-      <c r="B408" t="s">
-        <v>516</v>
-      </c>
-      <c r="C408" t="s">
-        <v>517</v>
       </c>
       <c r="D408" t="s">
         <v>3</v>
@@ -11214,13 +11211,13 @@
     </row>
     <row r="409" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
+        <v>517</v>
+      </c>
+      <c r="B409" t="s">
+        <v>517</v>
+      </c>
+      <c r="C409" t="s">
         <v>518</v>
-      </c>
-      <c r="B409" t="s">
-        <v>518</v>
-      </c>
-      <c r="C409" t="s">
-        <v>519</v>
       </c>
       <c r="D409" t="s">
         <v>25</v>
@@ -11234,13 +11231,13 @@
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
+        <v>519</v>
+      </c>
+      <c r="B410" t="s">
+        <v>519</v>
+      </c>
+      <c r="C410" t="s">
         <v>520</v>
-      </c>
-      <c r="B410" t="s">
-        <v>520</v>
-      </c>
-      <c r="C410" t="s">
-        <v>521</v>
       </c>
       <c r="D410" t="s">
         <v>3</v>
@@ -11254,13 +11251,13 @@
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
+        <v>521</v>
+      </c>
+      <c r="B411" t="s">
+        <v>521</v>
+      </c>
+      <c r="C411" t="s">
         <v>522</v>
-      </c>
-      <c r="B411" t="s">
-        <v>522</v>
-      </c>
-      <c r="C411" t="s">
-        <v>523</v>
       </c>
       <c r="D411" t="s">
         <v>3</v>
@@ -11274,13 +11271,13 @@
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
+        <v>523</v>
+      </c>
+      <c r="B412" t="s">
+        <v>523</v>
+      </c>
+      <c r="C412" t="s">
         <v>524</v>
-      </c>
-      <c r="B412" t="s">
-        <v>524</v>
-      </c>
-      <c r="C412" t="s">
-        <v>525</v>
       </c>
       <c r="D412" t="s">
         <v>3</v>
@@ -11294,13 +11291,13 @@
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
+        <v>526</v>
+      </c>
+      <c r="B413" t="s">
+        <v>526</v>
+      </c>
+      <c r="C413" t="s">
         <v>527</v>
-      </c>
-      <c r="B413" t="s">
-        <v>527</v>
-      </c>
-      <c r="C413" t="s">
-        <v>528</v>
       </c>
       <c r="D413" t="s">
         <v>105</v>
@@ -11314,13 +11311,13 @@
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B414" t="s">
+        <v>528</v>
+      </c>
+      <c r="C414" t="s">
         <v>529</v>
-      </c>
-      <c r="C414" t="s">
-        <v>530</v>
       </c>
       <c r="D414" t="s">
         <v>105</v>
@@ -11334,13 +11331,13 @@
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
+        <v>528</v>
+      </c>
+      <c r="B415" t="s">
+        <v>528</v>
+      </c>
+      <c r="C415" t="s">
         <v>529</v>
-      </c>
-      <c r="B415" t="s">
-        <v>529</v>
-      </c>
-      <c r="C415" t="s">
-        <v>530</v>
       </c>
       <c r="D415" t="s">
         <v>105</v>
@@ -11354,13 +11351,13 @@
     </row>
     <row r="416" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
+        <v>530</v>
+      </c>
+      <c r="B416" t="s">
+        <v>530</v>
+      </c>
+      <c r="C416" t="s">
         <v>531</v>
-      </c>
-      <c r="B416" t="s">
-        <v>531</v>
-      </c>
-      <c r="C416" t="s">
-        <v>532</v>
       </c>
       <c r="D416" t="s">
         <v>3</v>
@@ -11374,13 +11371,13 @@
     </row>
     <row r="417" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
+        <v>532</v>
+      </c>
+      <c r="B417" t="s">
+        <v>532</v>
+      </c>
+      <c r="C417" t="s">
         <v>533</v>
-      </c>
-      <c r="B417" t="s">
-        <v>533</v>
-      </c>
-      <c r="C417" t="s">
-        <v>534</v>
       </c>
       <c r="D417" t="s">
         <v>105</v>
@@ -11394,13 +11391,13 @@
     </row>
     <row r="418" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
+        <v>534</v>
+      </c>
+      <c r="B418" t="s">
+        <v>534</v>
+      </c>
+      <c r="C418" t="s">
         <v>535</v>
-      </c>
-      <c r="B418" t="s">
-        <v>535</v>
-      </c>
-      <c r="C418" t="s">
-        <v>536</v>
       </c>
       <c r="D418" t="s">
         <v>3</v>
@@ -11414,13 +11411,13 @@
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
+        <v>536</v>
+      </c>
+      <c r="B419" t="s">
+        <v>536</v>
+      </c>
+      <c r="C419" t="s">
         <v>537</v>
-      </c>
-      <c r="B419" t="s">
-        <v>537</v>
-      </c>
-      <c r="C419" t="s">
-        <v>538</v>
       </c>
       <c r="D419" t="s">
         <v>3</v>
@@ -11434,13 +11431,13 @@
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
+        <v>538</v>
+      </c>
+      <c r="B420" t="s">
+        <v>538</v>
+      </c>
+      <c r="C420" t="s">
         <v>539</v>
-      </c>
-      <c r="B420" t="s">
-        <v>539</v>
-      </c>
-      <c r="C420" t="s">
-        <v>540</v>
       </c>
       <c r="D420" t="s">
         <v>105</v>
@@ -11454,13 +11451,13 @@
     </row>
     <row r="421" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
+        <v>540</v>
+      </c>
+      <c r="B421" t="s">
+        <v>540</v>
+      </c>
+      <c r="C421" t="s">
         <v>541</v>
-      </c>
-      <c r="B421" t="s">
-        <v>541</v>
-      </c>
-      <c r="C421" t="s">
-        <v>542</v>
       </c>
       <c r="D421" t="s">
         <v>3</v>
@@ -11474,13 +11471,13 @@
     </row>
     <row r="422" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
+        <v>542</v>
+      </c>
+      <c r="B422" t="s">
+        <v>542</v>
+      </c>
+      <c r="C422" t="s">
         <v>543</v>
-      </c>
-      <c r="B422" t="s">
-        <v>543</v>
-      </c>
-      <c r="C422" t="s">
-        <v>544</v>
       </c>
       <c r="D422" t="s">
         <v>3</v>
@@ -11494,13 +11491,13 @@
     </row>
     <row r="423" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
+        <v>545</v>
+      </c>
+      <c r="B423" t="s">
+        <v>545</v>
+      </c>
+      <c r="C423" t="s">
         <v>546</v>
-      </c>
-      <c r="B423" t="s">
-        <v>546</v>
-      </c>
-      <c r="C423" t="s">
-        <v>547</v>
       </c>
       <c r="D423" t="s">
         <v>3</v>
@@ -11514,13 +11511,13 @@
     </row>
     <row r="424" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
+        <v>544</v>
+      </c>
+      <c r="B424" t="s">
         <v>545</v>
       </c>
-      <c r="B424" t="s">
+      <c r="C424" t="s">
         <v>546</v>
-      </c>
-      <c r="C424" t="s">
-        <v>547</v>
       </c>
       <c r="D424" t="s">
         <v>3</v>
@@ -11534,13 +11531,13 @@
     </row>
     <row r="425" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
+        <v>547</v>
+      </c>
+      <c r="B425" t="s">
+        <v>547</v>
+      </c>
+      <c r="C425" t="s">
         <v>548</v>
-      </c>
-      <c r="B425" t="s">
-        <v>548</v>
-      </c>
-      <c r="C425" t="s">
-        <v>549</v>
       </c>
       <c r="D425" t="s">
         <v>3</v>
@@ -11554,13 +11551,13 @@
     </row>
     <row r="426" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
+        <v>550</v>
+      </c>
+      <c r="B426" t="s">
+        <v>550</v>
+      </c>
+      <c r="C426" t="s">
         <v>551</v>
-      </c>
-      <c r="B426" t="s">
-        <v>551</v>
-      </c>
-      <c r="C426" t="s">
-        <v>552</v>
       </c>
       <c r="D426" t="s">
         <v>3</v>
@@ -11574,13 +11571,13 @@
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
+        <v>553</v>
+      </c>
+      <c r="B427" t="s">
+        <v>553</v>
+      </c>
+      <c r="C427" t="s">
         <v>554</v>
-      </c>
-      <c r="B427" t="s">
-        <v>554</v>
-      </c>
-      <c r="C427" t="s">
-        <v>555</v>
       </c>
       <c r="D427" t="s">
         <v>3</v>
@@ -11594,13 +11591,13 @@
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
+        <v>556</v>
+      </c>
+      <c r="B428" t="s">
+        <v>556</v>
+      </c>
+      <c r="C428" t="s">
         <v>557</v>
-      </c>
-      <c r="B428" t="s">
-        <v>557</v>
-      </c>
-      <c r="C428" t="s">
-        <v>558</v>
       </c>
       <c r="D428" t="s">
         <v>3</v>
@@ -11614,13 +11611,13 @@
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
+        <v>558</v>
+      </c>
+      <c r="B429" t="s">
+        <v>558</v>
+      </c>
+      <c r="C429" t="s">
         <v>559</v>
-      </c>
-      <c r="B429" t="s">
-        <v>559</v>
-      </c>
-      <c r="C429" t="s">
-        <v>560</v>
       </c>
       <c r="D429" t="s">
         <v>3</v>
@@ -11634,13 +11631,13 @@
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
+        <v>651</v>
+      </c>
+      <c r="B430" t="s">
+        <v>651</v>
+      </c>
+      <c r="C430" t="s">
         <v>652</v>
-      </c>
-      <c r="B430" t="s">
-        <v>652</v>
-      </c>
-      <c r="C430" t="s">
-        <v>653</v>
       </c>
       <c r="D430" t="s">
         <v>3</v>
@@ -11654,13 +11651,13 @@
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
+        <v>653</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="C431" t="s">
         <v>654</v>
-      </c>
-      <c r="B431" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="C431" t="s">
-        <v>655</v>
       </c>
       <c r="D431" t="s">
         <v>3</v>
@@ -11697,10 +11694,10 @@
         <v>161</v>
       </c>
       <c r="B433" t="s">
+        <v>453</v>
+      </c>
+      <c r="C433" t="s">
         <v>454</v>
-      </c>
-      <c r="C433" t="s">
-        <v>455</v>
       </c>
       <c r="D433" t="s">
         <v>3</v>
@@ -11714,13 +11711,13 @@
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B434" t="s">
+        <v>488</v>
+      </c>
+      <c r="C434" t="s">
         <v>489</v>
-      </c>
-      <c r="C434" t="s">
-        <v>490</v>
       </c>
       <c r="D434" t="s">
         <v>3</v>
@@ -11777,10 +11774,10 @@
         <v>88</v>
       </c>
       <c r="B437" t="s">
+        <v>473</v>
+      </c>
+      <c r="C437" t="s">
         <v>474</v>
-      </c>
-      <c r="C437" t="s">
-        <v>475</v>
       </c>
       <c r="D437" t="s">
         <v>3</v>
@@ -11797,10 +11794,10 @@
         <v>88</v>
       </c>
       <c r="B438" t="s">
+        <v>523</v>
+      </c>
+      <c r="C438" t="s">
         <v>524</v>
-      </c>
-      <c r="C438" t="s">
-        <v>525</v>
       </c>
       <c r="D438" t="s">
         <v>3</v>
@@ -11837,10 +11834,10 @@
         <v>89</v>
       </c>
       <c r="B440" t="s">
+        <v>523</v>
+      </c>
+      <c r="C440" t="s">
         <v>524</v>
-      </c>
-      <c r="C440" t="s">
-        <v>525</v>
       </c>
       <c r="D440" t="s">
         <v>3</v>
@@ -11877,10 +11874,10 @@
         <v>90</v>
       </c>
       <c r="B442" t="s">
+        <v>523</v>
+      </c>
+      <c r="C442" t="s">
         <v>524</v>
-      </c>
-      <c r="C442" t="s">
-        <v>525</v>
       </c>
       <c r="D442" t="s">
         <v>3</v>
@@ -11894,7 +11891,7 @@
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B443" t="s">
         <v>59</v>
@@ -11937,10 +11934,10 @@
         <v>91</v>
       </c>
       <c r="B445" t="s">
+        <v>523</v>
+      </c>
+      <c r="C445" t="s">
         <v>524</v>
-      </c>
-      <c r="C445" t="s">
-        <v>525</v>
       </c>
       <c r="D445" t="s">
         <v>3</v>
@@ -12054,7 +12051,7 @@
     </row>
     <row r="451" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B451" t="s">
         <v>132</v>
@@ -12074,13 +12071,13 @@
     </row>
     <row r="452" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B452" t="s">
+        <v>523</v>
+      </c>
+      <c r="C452" t="s">
         <v>524</v>
-      </c>
-      <c r="C452" t="s">
-        <v>525</v>
       </c>
       <c r="D452" t="s">
         <v>3</v>
@@ -12157,10 +12154,10 @@
         <v>96</v>
       </c>
       <c r="B456" t="s">
+        <v>523</v>
+      </c>
+      <c r="C456" t="s">
         <v>524</v>
-      </c>
-      <c r="C456" t="s">
-        <v>525</v>
       </c>
       <c r="D456" t="s">
         <v>3</v>
@@ -12174,13 +12171,13 @@
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
+        <v>560</v>
+      </c>
+      <c r="B457" t="s">
+        <v>560</v>
+      </c>
+      <c r="C457" t="s">
         <v>561</v>
-      </c>
-      <c r="B457" t="s">
-        <v>561</v>
-      </c>
-      <c r="C457" t="s">
-        <v>562</v>
       </c>
       <c r="D457" t="s">
         <v>3</v>
@@ -12194,13 +12191,13 @@
     </row>
     <row r="458" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
+        <v>562</v>
+      </c>
+      <c r="B458" t="s">
+        <v>562</v>
+      </c>
+      <c r="C458" t="s">
         <v>563</v>
-      </c>
-      <c r="B458" t="s">
-        <v>563</v>
-      </c>
-      <c r="C458" t="s">
-        <v>564</v>
       </c>
       <c r="D458" t="s">
         <v>3</v>
@@ -12214,13 +12211,13 @@
     </row>
     <row r="459" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
+        <v>564</v>
+      </c>
+      <c r="B459" t="s">
+        <v>564</v>
+      </c>
+      <c r="C459" t="s">
         <v>565</v>
-      </c>
-      <c r="B459" t="s">
-        <v>565</v>
-      </c>
-      <c r="C459" t="s">
-        <v>566</v>
       </c>
       <c r="D459" t="s">
         <v>3</v>
@@ -12234,13 +12231,13 @@
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
+        <v>566</v>
+      </c>
+      <c r="B460" t="s">
+        <v>566</v>
+      </c>
+      <c r="C460" t="s">
         <v>567</v>
-      </c>
-      <c r="B460" t="s">
-        <v>567</v>
-      </c>
-      <c r="C460" t="s">
-        <v>568</v>
       </c>
       <c r="D460" t="s">
         <v>3</v>
@@ -12254,13 +12251,13 @@
     </row>
     <row r="461" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
+        <v>568</v>
+      </c>
+      <c r="B461" t="s">
+        <v>568</v>
+      </c>
+      <c r="C461" t="s">
         <v>569</v>
-      </c>
-      <c r="B461" t="s">
-        <v>569</v>
-      </c>
-      <c r="C461" t="s">
-        <v>570</v>
       </c>
       <c r="D461" t="s">
         <v>3</v>
@@ -12274,13 +12271,13 @@
     </row>
     <row r="462" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
+        <v>570</v>
+      </c>
+      <c r="B462" t="s">
+        <v>570</v>
+      </c>
+      <c r="C462" t="s">
         <v>571</v>
-      </c>
-      <c r="B462" t="s">
-        <v>571</v>
-      </c>
-      <c r="C462" t="s">
-        <v>572</v>
       </c>
       <c r="D462" t="s">
         <v>105</v>
@@ -12294,13 +12291,13 @@
     </row>
     <row r="463" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B463" t="s">
+        <v>408</v>
+      </c>
+      <c r="C463" t="s">
         <v>409</v>
-      </c>
-      <c r="C463" t="s">
-        <v>410</v>
       </c>
       <c r="D463" t="s">
         <v>3</v>
@@ -12314,13 +12311,13 @@
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B464" t="s">
+        <v>408</v>
+      </c>
+      <c r="C464" t="s">
         <v>409</v>
-      </c>
-      <c r="C464" t="s">
-        <v>410</v>
       </c>
       <c r="D464" t="s">
         <v>3</v>
@@ -12334,7 +12331,7 @@
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B465" t="s">
         <v>132</v>
@@ -12354,13 +12351,13 @@
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B466" t="s">
+        <v>523</v>
+      </c>
+      <c r="C466" t="s">
         <v>524</v>
-      </c>
-      <c r="C466" t="s">
-        <v>525</v>
       </c>
       <c r="D466" t="s">
         <v>3</v>
@@ -12374,13 +12371,13 @@
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B467" t="s">
+        <v>488</v>
+      </c>
+      <c r="C467" t="s">
         <v>489</v>
-      </c>
-      <c r="C467" t="s">
-        <v>490</v>
       </c>
       <c r="D467" t="s">
         <v>3</v>
@@ -12394,13 +12391,13 @@
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B468" t="s">
+        <v>550</v>
+      </c>
+      <c r="C468" t="s">
         <v>551</v>
-      </c>
-      <c r="C468" t="s">
-        <v>552</v>
       </c>
       <c r="D468" t="s">
         <v>3</v>
@@ -12414,13 +12411,13 @@
     </row>
     <row r="469" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
+        <v>572</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C469" t="s">
         <v>573</v>
-      </c>
-      <c r="B469" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="C469" t="s">
-        <v>574</v>
       </c>
       <c r="D469" t="s">
         <v>3</v>
@@ -12434,13 +12431,13 @@
     </row>
     <row r="470" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
+        <v>574</v>
+      </c>
+      <c r="B470" t="s">
+        <v>574</v>
+      </c>
+      <c r="C470" t="s">
         <v>575</v>
-      </c>
-      <c r="B470" t="s">
-        <v>575</v>
-      </c>
-      <c r="C470" t="s">
-        <v>576</v>
       </c>
       <c r="D470" t="s">
         <v>3</v>
@@ -12454,13 +12451,13 @@
     </row>
     <row r="471" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
+        <v>576</v>
+      </c>
+      <c r="B471" t="s">
+        <v>576</v>
+      </c>
+      <c r="C471" t="s">
         <v>577</v>
-      </c>
-      <c r="B471" t="s">
-        <v>577</v>
-      </c>
-      <c r="C471" t="s">
-        <v>578</v>
       </c>
       <c r="D471" t="s">
         <v>3</v>
@@ -12474,13 +12471,13 @@
     </row>
     <row r="472" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
+        <v>578</v>
+      </c>
+      <c r="B472" t="s">
+        <v>578</v>
+      </c>
+      <c r="C472" t="s">
         <v>579</v>
-      </c>
-      <c r="B472" t="s">
-        <v>579</v>
-      </c>
-      <c r="C472" t="s">
-        <v>580</v>
       </c>
       <c r="D472" t="s">
         <v>3</v>
@@ -12494,13 +12491,13 @@
     </row>
     <row r="473" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
+        <v>580</v>
+      </c>
+      <c r="B473" t="s">
+        <v>580</v>
+      </c>
+      <c r="C473" t="s">
         <v>581</v>
-      </c>
-      <c r="B473" t="s">
-        <v>581</v>
-      </c>
-      <c r="C473" t="s">
-        <v>582</v>
       </c>
       <c r="D473" t="s">
         <v>3</v>
@@ -12514,13 +12511,13 @@
     </row>
     <row r="474" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
+        <v>582</v>
+      </c>
+      <c r="B474" t="s">
+        <v>582</v>
+      </c>
+      <c r="C474" t="s">
         <v>583</v>
-      </c>
-      <c r="B474" t="s">
-        <v>583</v>
-      </c>
-      <c r="C474" t="s">
-        <v>584</v>
       </c>
       <c r="D474" t="s">
         <v>3</v>
@@ -12534,13 +12531,13 @@
     </row>
     <row r="475" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
+        <v>584</v>
+      </c>
+      <c r="B475" t="s">
+        <v>584</v>
+      </c>
+      <c r="C475" t="s">
         <v>585</v>
-      </c>
-      <c r="B475" t="s">
-        <v>585</v>
-      </c>
-      <c r="C475" t="s">
-        <v>586</v>
       </c>
       <c r="D475" t="s">
         <v>3</v>

</xml_diff>